<commit_message>
atualização base de dados 02-07
</commit_message>
<xml_diff>
--- a/Cobertura_de_Carteira.xlsx
+++ b/Cobertura_de_Carteira.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\Kidy\Documentos\kIDY - mAPEAMENTOS\cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D493A2D8-39D8-4329-ADD5-337C2B9859C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C094B4C0-1081-43FA-B86D-55DF567B8773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2BD4FA7B-4EC3-4FF7-B70D-ACBAF1B8A7C0}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2BD4FA7B-4EC3-4FF7-B70D-ACBAF1B8A7C0}"/>
   </bookViews>
   <sheets>
     <sheet name="cobertura" sheetId="1" r:id="rId1"/>
@@ -328,7 +328,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -370,6 +370,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -379,7 +380,97 @@
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -398,38 +489,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -464,80 +523,10 @@
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -574,6 +563,108 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="14" formatCode="0.00%"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -819,36 +910,6 @@
           <color theme="4" tint="-0.499984740745262"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -937,7 +998,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:t>29/06/2025</a:t>
+            <a:t>01/07/2025</a:t>
           </a:fld>
           <a:endParaRPr lang="pt-BR" sz="1100" b="1">
             <a:solidFill>
@@ -1411,7 +1472,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:t>29,71%</a:t>
+            <a:t>32,82%</a:t>
           </a:fld>
           <a:endParaRPr lang="pt-BR" sz="1100" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -2291,6 +2352,7 @@
       <sheetName val="NOVA CARTEIRA"/>
       <sheetName val="ATENDIDOS 2025"/>
       <sheetName val="Ausentes (3)"/>
+      <sheetName val="Planilha7"/>
       <sheetName val="cobertura"/>
       <sheetName val="Ausentes"/>
       <sheetName val="Planilha6"/>
@@ -2314,40 +2376,41 @@
       <sheetName val="Planilha5"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6">
         <row r="23">
           <cell r="D23">
-            <v>7355</v>
+            <v>7144</v>
           </cell>
           <cell r="E23">
-            <v>1233</v>
+            <v>1227</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2370,26 +2433,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C699080-BB77-4B73-A408-C4AABE6B398B}" name="Tabela1" displayName="Tabela1" ref="A8:M60" totalsRowCount="1" headerRowDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C699080-BB77-4B73-A408-C4AABE6B398B}" name="Tabela1" displayName="Tabela1" ref="A8:M60" totalsRowCount="1" headerRowDxfId="27" tableBorderDxfId="26">
   <autoFilter ref="A8:M59" xr:uid="{2C699080-BB77-4B73-A408-C4AABE6B398B}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{2E103CB5-8552-4DFF-8DFF-D7107D28CA72}" name="Rep" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{DC53BAE2-FEFB-4577-8C31-8C708160F4AE}" name="Nome Rep." dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{98443E25-9A69-4DD4-BEF1-083F32064E92}" name="Supervisor" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{313671CC-B700-48CF-9572-F301644DDCBF}" name="Carteira" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{99AB9EB0-9D28-4F16-99B2-865263D09091}" name="Bloqueados" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{3F77B725-1A7B-4337-AFEC-F2B0738A84A9}" name="Abertos 2025 2º SEM" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{B161C5DE-CB19-4197-B530-CF605C61AEE8}" name="Sem Limite" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{7DF927DB-FC14-493C-8860-08E3337FCB7E}" name="Saldo de Carteira" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{2E103CB5-8552-4DFF-8DFF-D7107D28CA72}" name="Rep" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{DC53BAE2-FEFB-4577-8C31-8C708160F4AE}" name="Nome Rep." dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{98443E25-9A69-4DD4-BEF1-083F32064E92}" name="Supervisor" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{313671CC-B700-48CF-9572-F301644DDCBF}" name="Carteira" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{99AB9EB0-9D28-4F16-99B2-865263D09091}" name="Bloqueados" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{3F77B725-1A7B-4337-AFEC-F2B0738A84A9}" name="Abertos 2025 2º SEM" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{B161C5DE-CB19-4197-B530-CF605C61AEE8}" name="Sem Limite" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{7DF927DB-FC14-493C-8860-08E3337FCB7E}" name="Saldo de Carteira" dataDxfId="18">
       <calculatedColumnFormula>D9-E9+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{39FC1898-2573-42E0-BC52-C9F93D1A1B69}" name="cobertura" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{73729B4D-016C-45AC-84B0-5F4C6E582133}" name="% Cobertura" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Normal">
+    <tableColumn id="5" xr3:uid="{39FC1898-2573-42E0-BC52-C9F93D1A1B69}" name="cobertura" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{73729B4D-016C-45AC-84B0-5F4C6E582133}" name="% Cobertura" dataDxfId="16" totalsRowDxfId="12" dataCellStyle="Normal">
       <calculatedColumnFormula>I9/H9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{DB269E38-4E7F-4032-855F-5F7E2DDD3628}" name="mix" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{5E7F18D1-3A42-4F78-BD2B-40CF376728D7}" name="Meta Cob. Dia Crianças" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{0BC7EA2F-5567-46FC-9D2B-47B38F66221B}" name="Meta Cob. Coleção" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="7" xr3:uid="{DB269E38-4E7F-4032-855F-5F7E2DDD3628}" name="mix" dataDxfId="15" totalsRowDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{5E7F18D1-3A42-4F78-BD2B-40CF376728D7}" name="Meta Cob. Dia Crianças" dataDxfId="14" totalsRowDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{0BC7EA2F-5567-46FC-9D2B-47B38F66221B}" name="Meta Cob. Coleção" dataDxfId="13" totalsRowDxfId="9">
       <calculatedColumnFormula>Tabela1[[#This Row],[Saldo de Carteira]]*80%</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2697,8 +2760,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,7 +2795,7 @@
       <c r="M2" s="26"/>
       <c r="P2" s="13">
         <f ca="1">TODAY()-1</f>
-        <v>45837</v>
+        <v>45839</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2750,41 +2813,41 @@
     <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E5" s="16">
         <f>E6/D6</f>
-        <v>4.8181576851606053E-2</v>
+        <v>4.1603526656564263E-2</v>
       </c>
       <c r="F5" s="16">
         <f>F6/D6</f>
-        <v>2.4555349084151846E-2</v>
+        <v>2.5898884143821462E-2</v>
       </c>
       <c r="G5" s="16">
         <f>G6/D6</f>
-        <v>2.3626227767454207E-2</v>
+        <v>2.4521283923405426E-2</v>
       </c>
       <c r="J5" s="28">
         <f>J6-'% cOB. caRT'!D9</f>
-        <v>-0.12948317847601484</v>
+        <v>-0.15651579335359697</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="26"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="2">
         <f>SUBTOTAL(9,Tabela1[Carteira])</f>
-        <v>7534</v>
+        <v>7259</v>
       </c>
       <c r="E6" s="2">
         <f>SUBTOTAL(9,Tabela1[Bloqueados])</f>
-        <v>363</v>
+        <v>302</v>
       </c>
       <c r="F6" s="2">
         <f>SUBTOTAL(9,Tabela1[Abertos 2025 2º SEM])</f>
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G6" s="2">
         <f>SUBTOTAL(9,Tabela1[Sem Limite])</f>
@@ -2792,15 +2855,15 @@
       </c>
       <c r="H6" s="2">
         <f>SUBTOTAL(9,Tabela1[Saldo de Carteira])</f>
-        <v>7356</v>
+        <v>7145</v>
       </c>
       <c r="I6" s="2">
         <f>SUBTOTAL(9,Tabela1[cobertura])</f>
-        <v>1233</v>
+        <v>1227</v>
       </c>
       <c r="J6" s="28">
         <f>I6/H6</f>
-        <v>0.16761827079934746</v>
+        <v>0.17172848145556333</v>
       </c>
       <c r="K6" s="3">
         <f>SUBTOTAL(101,Tabela1[mix])</f>
@@ -2877,11 +2940,10 @@
         <v>9902</v>
       </c>
       <c r="D9" s="8">
-        <f>252-27</f>
-        <v>225</v>
+        <v>142</v>
       </c>
       <c r="E9" s="8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F9" s="8">
         <v>1</v>
@@ -2891,14 +2953,14 @@
       </c>
       <c r="H9" s="8">
         <f>D9-E9+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>219</v>
+        <v>138</v>
       </c>
       <c r="I9" s="8">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="J9" s="12">
         <f t="shared" ref="J9:J59" si="0">I9/H9</f>
-        <v>0.15981735159817351</v>
+        <v>9.420289855072464E-2</v>
       </c>
       <c r="K9" s="10">
         <v>14.92</v>
@@ -2906,7 +2968,7 @@
       <c r="L9" s="10"/>
       <c r="M9" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>175.20000000000002</v>
+        <v>110.4</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2924,7 +2986,7 @@
         <v>175</v>
       </c>
       <c r="E10" s="8">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F10" s="8">
         <v>5</v>
@@ -2934,14 +2996,14 @@
       </c>
       <c r="H10" s="8">
         <f>D10-E10+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="I10" s="8">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J10" s="12">
         <f t="shared" si="0"/>
-        <v>0.22500000000000001</v>
+        <v>0.29878048780487804</v>
       </c>
       <c r="K10" s="10">
         <v>12.53</v>
@@ -2949,7 +3011,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>128</v>
+        <v>131.20000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2967,7 +3029,7 @@
         <v>111</v>
       </c>
       <c r="E11" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" s="8">
         <v>0</v>
@@ -2977,14 +3039,14 @@
       </c>
       <c r="H11" s="8">
         <f>D11-E11+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I11" s="8">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J11" s="12">
         <f t="shared" si="0"/>
-        <v>0.22857142857142856</v>
+        <v>0.23584905660377359</v>
       </c>
       <c r="K11" s="10">
         <v>12.53</v>
@@ -2992,7 +3054,7 @@
       <c r="L11" s="10"/>
       <c r="M11" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>84</v>
+        <v>84.800000000000011</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3010,7 +3072,7 @@
         <v>184</v>
       </c>
       <c r="E12" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="8">
         <v>11</v>
@@ -3020,14 +3082,14 @@
       </c>
       <c r="H12" s="8">
         <f>D12-E12+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I12" s="8">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J12" s="12">
         <f t="shared" si="0"/>
-        <v>0.32972972972972975</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K12" s="10">
         <v>7.87</v>
@@ -3035,7 +3097,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>148</v>
+        <v>148.80000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3053,7 +3115,7 @@
         <v>145</v>
       </c>
       <c r="E13" s="8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F13" s="8">
         <v>3</v>
@@ -3063,14 +3125,14 @@
       </c>
       <c r="H13" s="8">
         <f>D13-E13+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I13" s="8">
         <v>16</v>
       </c>
       <c r="J13" s="12">
         <f t="shared" si="0"/>
-        <v>0.11347517730496454</v>
+        <v>0.11188811188811189</v>
       </c>
       <c r="K13" s="10">
         <v>8.75</v>
@@ -3078,7 +3140,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>112.80000000000001</v>
+        <v>114.4</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3097,7 +3159,7 @@
         <v>126</v>
       </c>
       <c r="E14" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" s="8">
         <v>0</v>
@@ -3107,14 +3169,14 @@
       </c>
       <c r="H14" s="8">
         <f>D14-E14+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I14" s="8">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J14" s="12">
         <f t="shared" si="0"/>
-        <v>0.27049180327868855</v>
+        <v>0.27642276422764228</v>
       </c>
       <c r="K14" s="10">
         <v>12.4</v>
@@ -3122,7 +3184,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>97.600000000000009</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3153,11 +3215,11 @@
         <v>146</v>
       </c>
       <c r="I15" s="8">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J15" s="12">
         <f t="shared" si="0"/>
-        <v>0.13013698630136986</v>
+        <v>0.16438356164383561</v>
       </c>
       <c r="K15" s="10">
         <v>11.9</v>
@@ -3186,21 +3248,21 @@
         <v>10</v>
       </c>
       <c r="F16" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G16" s="14">
         <v>2</v>
       </c>
       <c r="H16" s="8">
         <f>D16-E16+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I16" s="8">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J16" s="12">
         <f t="shared" si="0"/>
-        <v>0.28846153846153844</v>
+        <v>0.29523809523809524</v>
       </c>
       <c r="K16" s="10">
         <v>4.76</v>
@@ -3208,7 +3270,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>83.2</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -3226,7 +3288,7 @@
         <v>64</v>
       </c>
       <c r="E17" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" s="8">
         <v>3</v>
@@ -3236,14 +3298,14 @@
       </c>
       <c r="H17" s="8">
         <f>D17-E17+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I17" s="8">
         <v>14</v>
       </c>
       <c r="J17" s="12">
         <f t="shared" si="0"/>
-        <v>0.21875</v>
+        <v>0.2153846153846154</v>
       </c>
       <c r="K17" s="10">
         <v>6.17</v>
@@ -3251,7 +3313,7 @@
       <c r="L17" s="10"/>
       <c r="M17" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>51.2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3282,11 +3344,11 @@
         <v>224</v>
       </c>
       <c r="I18" s="8">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="J18" s="12">
         <f t="shared" si="0"/>
-        <v>0.26339285714285715</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="K18" s="10">
         <v>10.050000000000001</v>
@@ -3312,7 +3374,7 @@
         <v>93</v>
       </c>
       <c r="E19" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" s="8">
         <v>4</v>
@@ -3322,14 +3384,14 @@
       </c>
       <c r="H19" s="8">
         <f>D19-E19+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I19" s="8">
         <v>30</v>
       </c>
       <c r="J19" s="12">
         <f t="shared" si="0"/>
-        <v>0.32258064516129031</v>
+        <v>0.31914893617021278</v>
       </c>
       <c r="K19" s="10">
         <v>4.4800000000000004</v>
@@ -3337,7 +3399,7 @@
       <c r="L19" s="10"/>
       <c r="M19" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>74.400000000000006</v>
+        <v>75.2</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3412,11 +3474,11 @@
         <v>155</v>
       </c>
       <c r="I21" s="8">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="J21" s="12">
         <f t="shared" si="0"/>
-        <v>0.36774193548387096</v>
+        <v>0.16774193548387098</v>
       </c>
       <c r="K21" s="10">
         <v>11.67</v>
@@ -3442,24 +3504,24 @@
         <v>159</v>
       </c>
       <c r="E22" s="8">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F22" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G22" s="14">
         <v>4</v>
       </c>
       <c r="H22" s="8">
         <f>D22-E22+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="I22" s="8">
         <v>16</v>
       </c>
       <c r="J22" s="12">
         <f t="shared" si="0"/>
-        <v>0.1038961038961039</v>
+        <v>0.10191082802547771</v>
       </c>
       <c r="K22" s="10">
         <v>4.82</v>
@@ -3467,7 +3529,7 @@
       <c r="L22" s="10"/>
       <c r="M22" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>123.2</v>
+        <v>125.60000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3486,7 +3548,7 @@
         <v>158</v>
       </c>
       <c r="E23" s="8">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F23" s="8">
         <v>8</v>
@@ -3496,14 +3558,14 @@
       </c>
       <c r="H23" s="8">
         <f>D23-E23+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="I23" s="8">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J23" s="12">
         <f t="shared" si="0"/>
-        <v>0.18064516129032257</v>
+        <v>0.189873417721519</v>
       </c>
       <c r="K23" s="10">
         <v>7.5</v>
@@ -3511,7 +3573,7 @@
       <c r="L23" s="10"/>
       <c r="M23" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>124</v>
+        <v>126.4</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3529,7 +3591,7 @@
         <v>229</v>
       </c>
       <c r="E24" s="8">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F24" s="8">
         <v>11</v>
@@ -3539,14 +3601,14 @@
       </c>
       <c r="H24" s="8">
         <f>D24-E24+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="I24" s="8">
         <v>49</v>
       </c>
       <c r="J24" s="12">
         <f t="shared" si="0"/>
-        <v>0.21973094170403587</v>
+        <v>0.21777777777777776</v>
       </c>
       <c r="K24" s="10">
         <v>9.52</v>
@@ -3554,7 +3616,7 @@
       <c r="L24" s="10"/>
       <c r="M24" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>178.4</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -3572,7 +3634,7 @@
         <v>106</v>
       </c>
       <c r="E25" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" s="8">
         <v>0</v>
@@ -3582,14 +3644,14 @@
       </c>
       <c r="H25" s="8">
         <f>D25-E25+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I25" s="8">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J25" s="12">
         <f t="shared" si="0"/>
-        <v>0.27</v>
+        <v>0.28712871287128711</v>
       </c>
       <c r="K25" s="10">
         <v>7.29</v>
@@ -3597,7 +3659,7 @@
       <c r="L25" s="10"/>
       <c r="M25" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>80</v>
+        <v>80.800000000000011</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3616,7 +3678,7 @@
         <v>91</v>
       </c>
       <c r="E26" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" s="8">
         <v>0</v>
@@ -3626,14 +3688,14 @@
       </c>
       <c r="H26" s="8">
         <f>D26-E26+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I26" s="8">
         <v>12</v>
       </c>
       <c r="J26" s="12">
         <f t="shared" si="0"/>
-        <v>0.13636363636363635</v>
+        <v>0.1348314606741573</v>
       </c>
       <c r="K26" s="10">
         <v>7.29</v>
@@ -3641,7 +3703,7 @@
       <c r="L26" s="10"/>
       <c r="M26" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>70.400000000000006</v>
+        <v>71.2</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3659,7 +3721,7 @@
         <v>119</v>
       </c>
       <c r="E27" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="8">
         <v>5</v>
@@ -3669,14 +3731,14 @@
       </c>
       <c r="H27" s="8">
         <f>D27-E27+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I27" s="8">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J27" s="12">
         <f t="shared" si="0"/>
-        <v>0.2032520325203252</v>
+        <v>0.21311475409836064</v>
       </c>
       <c r="K27" s="10">
         <v>8.33</v>
@@ -3684,7 +3746,7 @@
       <c r="L27" s="10"/>
       <c r="M27" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>98.4</v>
+        <v>97.600000000000009</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3701,7 +3763,7 @@
         <v>178</v>
       </c>
       <c r="E28" s="8">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F28" s="8">
         <v>5</v>
@@ -3711,14 +3773,14 @@
       </c>
       <c r="H28" s="8">
         <f>D28-E28+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="I28" s="8">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J28" s="12">
         <f t="shared" si="0"/>
-        <v>0.30057803468208094</v>
+        <v>0.29943502824858759</v>
       </c>
       <c r="K28" s="10">
         <v>7.33</v>
@@ -3726,7 +3788,7 @@
       <c r="L28" s="10"/>
       <c r="M28" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>138.4</v>
+        <v>141.6</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3744,7 +3806,7 @@
         <v>127</v>
       </c>
       <c r="E29" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" s="8">
         <v>0</v>
@@ -3754,14 +3816,14 @@
       </c>
       <c r="H29" s="8">
         <f>D29-E29+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I29" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J29" s="12">
         <f t="shared" si="0"/>
-        <v>8.943089430894309E-2</v>
+        <v>9.6774193548387094E-2</v>
       </c>
       <c r="K29" s="10">
         <v>11</v>
@@ -3769,7 +3831,7 @@
       <c r="L29" s="10"/>
       <c r="M29" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>98.4</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3787,24 +3849,24 @@
         <v>257</v>
       </c>
       <c r="E30" s="8">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F30" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G30" s="14">
         <v>1</v>
       </c>
       <c r="H30" s="8">
         <f>D30-E30+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="I30" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J30" s="12">
         <f t="shared" si="0"/>
-        <v>3.968253968253968E-2</v>
+        <v>4.296875E-2</v>
       </c>
       <c r="K30" s="10">
         <v>7.5</v>
@@ -3812,7 +3874,7 @@
       <c r="L30" s="10"/>
       <c r="M30" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>201.60000000000002</v>
+        <v>204.8</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -3830,7 +3892,7 @@
         <v>140</v>
       </c>
       <c r="E31" s="8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F31" s="8">
         <v>0</v>
@@ -3840,14 +3902,14 @@
       </c>
       <c r="H31" s="8">
         <f>D31-E31+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I31" s="8">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J31" s="12">
         <f t="shared" si="0"/>
-        <v>0.26315789473684209</v>
+        <v>0.2814814814814815</v>
       </c>
       <c r="K31" s="10">
         <v>6.54</v>
@@ -3855,7 +3917,7 @@
       <c r="L31" s="10"/>
       <c r="M31" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>106.4</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3873,7 +3935,7 @@
         <v>117</v>
       </c>
       <c r="E32" s="8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F32" s="8">
         <v>0</v>
@@ -3883,14 +3945,14 @@
       </c>
       <c r="H32" s="8">
         <f>D32-E32+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I32" s="8">
         <v>10</v>
       </c>
       <c r="J32" s="12">
         <f t="shared" si="0"/>
-        <v>9.0090090090090086E-2</v>
+        <v>9.1743119266055051E-2</v>
       </c>
       <c r="K32" s="10">
         <v>16.13</v>
@@ -3898,7 +3960,7 @@
       <c r="L32" s="10"/>
       <c r="M32" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>88.800000000000011</v>
+        <v>87.2</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3959,7 +4021,7 @@
         <v>177</v>
       </c>
       <c r="E34" s="8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F34" s="8">
         <v>5</v>
@@ -3969,14 +4031,14 @@
       </c>
       <c r="H34" s="8">
         <f>D34-E34+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="I34" s="8">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J34" s="12">
         <f t="shared" si="0"/>
-        <v>0.22857142857142856</v>
+        <v>0.2303370786516854</v>
       </c>
       <c r="K34" s="10">
         <v>6.59</v>
@@ -3984,7 +4046,7 @@
       <c r="L34" s="10"/>
       <c r="M34" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>140</v>
+        <v>142.4</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4002,7 +4064,7 @@
         <v>122</v>
       </c>
       <c r="E35" s="8">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F35" s="8">
         <v>1</v>
@@ -4012,14 +4074,14 @@
       </c>
       <c r="H35" s="8">
         <f>D35-E35+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="I35" s="8">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J35" s="12">
         <f t="shared" si="0"/>
-        <v>0.31858407079646017</v>
+        <v>0.33620689655172414</v>
       </c>
       <c r="K35" s="10">
         <v>8.8699999999999992</v>
@@ -4027,7 +4089,7 @@
       <c r="L35" s="10"/>
       <c r="M35" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>90.4</v>
+        <v>92.800000000000011</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4045,7 +4107,7 @@
         <v>272</v>
       </c>
       <c r="E36" s="8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F36" s="8">
         <v>4</v>
@@ -4055,14 +4117,14 @@
       </c>
       <c r="H36" s="8">
         <f>D36-E36+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="I36" s="8">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J36" s="12">
         <f t="shared" si="0"/>
-        <v>0.14772727272727273</v>
+        <v>0.15037593984962405</v>
       </c>
       <c r="K36" s="10">
         <v>10.37</v>
@@ -4070,7 +4132,7 @@
       <c r="L36" s="10"/>
       <c r="M36" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>211.20000000000002</v>
+        <v>212.8</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4088,7 +4150,7 @@
         <v>173</v>
       </c>
       <c r="E37" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" s="8">
         <v>3</v>
@@ -4098,14 +4160,14 @@
       </c>
       <c r="H37" s="8">
         <f>D37-E37+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I37" s="8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J37" s="12">
         <f t="shared" si="0"/>
-        <v>8.771929824561403E-2</v>
+        <v>9.3023255813953487E-2</v>
       </c>
       <c r="K37" s="10">
         <v>4.93</v>
@@ -4113,7 +4175,7 @@
       <c r="L37" s="10"/>
       <c r="M37" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>136.80000000000001</v>
+        <v>137.6</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4130,7 +4192,7 @@
         <v>134</v>
       </c>
       <c r="E38" s="8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F38" s="8">
         <v>0</v>
@@ -4140,14 +4202,14 @@
       </c>
       <c r="H38" s="8">
         <f>D38-E38+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I38" s="8">
         <v>10</v>
       </c>
       <c r="J38" s="12">
         <f t="shared" si="0"/>
-        <v>8.4033613445378158E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="K38" s="10">
         <v>6</v>
@@ -4155,7 +4217,7 @@
       <c r="L38" s="10"/>
       <c r="M38" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>95.2</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4173,7 +4235,7 @@
         <v>168</v>
       </c>
       <c r="E39" s="8">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F39" s="8">
         <v>1</v>
@@ -4183,14 +4245,14 @@
       </c>
       <c r="H39" s="8">
         <f>D39-E39+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="I39" s="8">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J39" s="12">
         <f t="shared" si="0"/>
-        <v>0.18867924528301888</v>
+        <v>0.20858895705521471</v>
       </c>
       <c r="K39" s="10">
         <v>6.23</v>
@@ -4198,7 +4260,7 @@
       <c r="L39" s="10"/>
       <c r="M39" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>127.2</v>
+        <v>130.4</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4216,7 +4278,7 @@
         <v>317</v>
       </c>
       <c r="E40" s="8">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F40" s="8">
         <v>2</v>
@@ -4226,14 +4288,14 @@
       </c>
       <c r="H40" s="8">
         <f>D40-E40+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I40" s="8">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J40" s="12">
         <f t="shared" si="0"/>
-        <v>5.921052631578947E-2</v>
+        <v>6.535947712418301E-2</v>
       </c>
       <c r="K40" s="10">
         <v>7.69</v>
@@ -4241,7 +4303,7 @@
       <c r="L40" s="10"/>
       <c r="M40" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>243.20000000000002</v>
+        <v>244.8</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4259,7 +4321,7 @@
         <v>130</v>
       </c>
       <c r="E41" s="8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F41" s="8">
         <v>3</v>
@@ -4269,14 +4331,14 @@
       </c>
       <c r="H41" s="8">
         <f>D41-E41+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I41" s="8">
         <v>26</v>
       </c>
       <c r="J41" s="12">
         <f t="shared" si="0"/>
-        <v>0.20634920634920634</v>
+        <v>0.203125</v>
       </c>
       <c r="K41" s="10">
         <v>8.8699999999999992</v>
@@ -4284,7 +4346,7 @@
       <c r="L41" s="10"/>
       <c r="M41" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>100.80000000000001</v>
+        <v>102.4</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4345,7 +4407,7 @@
         <v>206</v>
       </c>
       <c r="E43" s="8">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F43" s="8">
         <v>0</v>
@@ -4355,14 +4417,14 @@
       </c>
       <c r="H43" s="8">
         <f>D43-E43+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I43" s="8">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J43" s="12">
         <f t="shared" si="0"/>
-        <v>0.10240963855421686</v>
+        <v>0.11904761904761904</v>
       </c>
       <c r="K43" s="10">
         <v>6.65</v>
@@ -4370,7 +4432,7 @@
       <c r="L43" s="10"/>
       <c r="M43" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>132.80000000000001</v>
+        <v>134.4</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4388,7 +4450,7 @@
         <v>213</v>
       </c>
       <c r="E44" s="8">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F44" s="8">
         <v>7</v>
@@ -4398,14 +4460,14 @@
       </c>
       <c r="H44" s="8">
         <f>D44-E44+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="I44" s="8">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J44" s="12">
         <f t="shared" si="0"/>
-        <v>0.1941747572815534</v>
+        <v>0.19711538461538461</v>
       </c>
       <c r="K44" s="10">
         <v>4.62</v>
@@ -4413,7 +4475,7 @@
       <c r="L44" s="10"/>
       <c r="M44" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>164.8</v>
+        <v>166.4</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4474,7 +4536,7 @@
         <v>103</v>
       </c>
       <c r="E46" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" s="8">
         <v>0</v>
@@ -4484,14 +4546,14 @@
       </c>
       <c r="H46" s="8">
         <f>D46-E46+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I46" s="8">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J46" s="12">
         <f t="shared" si="0"/>
-        <v>0.13861386138613863</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="K46" s="10">
         <v>5.92</v>
@@ -4499,7 +4561,7 @@
       <c r="L46" s="10"/>
       <c r="M46" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>80.800000000000011</v>
+        <v>81.600000000000009</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -4516,7 +4578,7 @@
         <v>162</v>
       </c>
       <c r="E47" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" s="8">
         <v>1</v>
@@ -4526,14 +4588,14 @@
       </c>
       <c r="H47" s="8">
         <f>D47-E47+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I47" s="8">
         <v>10</v>
       </c>
       <c r="J47" s="12">
         <f t="shared" si="0"/>
-        <v>6.1728395061728392E-2</v>
+        <v>6.1349693251533742E-2</v>
       </c>
       <c r="K47" s="10">
         <v>3.75</v>
@@ -4541,7 +4603,7 @@
       <c r="L47" s="10"/>
       <c r="M47" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>129.6</v>
+        <v>130.4</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4558,7 +4620,7 @@
         <v>147</v>
       </c>
       <c r="E48" s="8">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F48" s="8">
         <v>3</v>
@@ -4568,14 +4630,14 @@
       </c>
       <c r="H48" s="8">
         <f>D48-E48+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="I48" s="8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J48" s="12">
         <f t="shared" si="0"/>
-        <v>0.10169491525423729</v>
+        <v>0.10743801652892562</v>
       </c>
       <c r="K48" s="10">
         <v>7.3</v>
@@ -4583,7 +4645,7 @@
       <c r="L48" s="10"/>
       <c r="M48" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>94.4</v>
+        <v>96.800000000000011</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -4601,7 +4663,7 @@
         <v>117</v>
       </c>
       <c r="E49" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="8">
         <v>2</v>
@@ -4611,14 +4673,14 @@
       </c>
       <c r="H49" s="8">
         <f>D49-E49+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I49" s="8">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J49" s="12">
         <f t="shared" si="0"/>
-        <v>0.25423728813559321</v>
+        <v>0.26050420168067229</v>
       </c>
       <c r="K49" s="10">
         <v>5.19</v>
@@ -4626,7 +4688,7 @@
       <c r="L49" s="10"/>
       <c r="M49" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>94.4</v>
+        <v>95.2</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4644,7 +4706,7 @@
         <v>136</v>
       </c>
       <c r="E50" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50" s="8">
         <v>3</v>
@@ -4654,14 +4716,14 @@
       </c>
       <c r="H50" s="8">
         <f>D50-E50+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I50" s="8">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J50" s="12">
         <f t="shared" si="0"/>
-        <v>0.10869565217391304</v>
+        <v>0.1223021582733813</v>
       </c>
       <c r="K50" s="10">
         <v>7.4</v>
@@ -4669,7 +4731,7 @@
       <c r="L50" s="10"/>
       <c r="M50" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>110.4</v>
+        <v>111.2</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4701,11 +4763,11 @@
         <v>110</v>
       </c>
       <c r="I51" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J51" s="12">
         <f t="shared" si="0"/>
-        <v>3.6363636363636362E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="K51" s="10">
         <v>15</v>
@@ -4745,11 +4807,11 @@
         <v>78</v>
       </c>
       <c r="I52" s="8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J52" s="12">
         <f t="shared" si="0"/>
-        <v>0.19230769230769232</v>
+        <v>0.20512820512820512</v>
       </c>
       <c r="K52" s="10">
         <v>6.5</v>
@@ -4774,7 +4836,7 @@
         <v>135</v>
       </c>
       <c r="E53" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" s="8">
         <v>2</v>
@@ -4784,14 +4846,14 @@
       </c>
       <c r="H53" s="8">
         <f>D53-E53+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I53" s="8">
         <v>23</v>
       </c>
       <c r="J53" s="12">
         <f t="shared" si="0"/>
-        <v>0.17424242424242425</v>
+        <v>0.17293233082706766</v>
       </c>
       <c r="K53" s="10">
         <v>7.91</v>
@@ -4799,7 +4861,7 @@
       <c r="L53" s="10"/>
       <c r="M53" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>105.60000000000001</v>
+        <v>106.4</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4897,7 +4959,7 @@
         <v>122</v>
       </c>
       <c r="E56" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" s="8">
         <v>2</v>
@@ -4907,14 +4969,14 @@
       </c>
       <c r="H56" s="8">
         <f>D56-E56+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I56" s="8">
         <v>40</v>
       </c>
       <c r="J56" s="12">
         <f t="shared" si="0"/>
-        <v>0.33057851239669422</v>
+        <v>0.32786885245901637</v>
       </c>
       <c r="K56" s="10">
         <v>4.58</v>
@@ -4922,7 +4984,7 @@
       <c r="L56" s="10"/>
       <c r="M56" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>96.800000000000011</v>
+        <v>97.600000000000009</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4940,7 +5002,7 @@
         <v>36</v>
       </c>
       <c r="E57" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" s="8">
         <v>20</v>
@@ -4950,14 +5012,14 @@
       </c>
       <c r="H57" s="8">
         <f>D57-E57+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I57" s="8">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J57" s="12">
         <f t="shared" si="0"/>
-        <v>0.28846153846153844</v>
+        <v>0.32075471698113206</v>
       </c>
       <c r="K57" s="10">
         <v>6.36</v>
@@ -4965,7 +5027,7 @@
       <c r="L57" s="10"/>
       <c r="M57" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>41.6</v>
+        <v>42.400000000000006</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4979,7 +5041,7 @@
         <v>9902</v>
       </c>
       <c r="D58" s="8">
-        <v>265</v>
+        <v>73</v>
       </c>
       <c r="E58" s="8">
         <v>0</v>
@@ -4992,14 +5054,14 @@
       </c>
       <c r="H58" s="8">
         <f>D58-E58+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>270</v>
+        <v>78</v>
       </c>
       <c r="I58" s="8">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="J58" s="12">
         <f t="shared" si="0"/>
-        <v>0.10740740740740741</v>
+        <v>0.14102564102564102</v>
       </c>
       <c r="K58" s="10">
         <v>9.56</v>
@@ -5007,7 +5069,7 @@
       <c r="L58" s="10"/>
       <c r="M58" s="29">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>216</v>
+        <v>62.400000000000006</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5066,17 +5128,17 @@
     <mergeCell ref="A6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
-      <formula>0.29</formula>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+      <formula>0.328</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J60">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="lessThan">
-      <formula>0.1499</formula>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
+      <formula>0.1699</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="between">
-      <formula>0.15</formula>
-      <formula>0.2999</formula>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
+      <formula>0.17</formula>
+      <formula>0.3279</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:L59">
@@ -5153,8 +5215,12 @@
         <v>21</v>
       </c>
       <c r="D2">
-        <f>SUM(B2:B8)</f>
-        <v>138</v>
+        <f>SUM(B8:B13)</f>
+        <v>131</v>
+      </c>
+      <c r="E2" s="25">
+        <f>D1/D2</f>
+        <v>7.6335877862595417E-3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5165,8 +5231,8 @@
         <v>16</v>
       </c>
       <c r="D3" s="25">
-        <f>D1/D2</f>
-        <v>7.246376811594203E-3</v>
+        <f>E2*D7</f>
+        <v>0.3282442748091603</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5188,8 +5254,8 @@
         <v>20</v>
       </c>
       <c r="D5">
-        <f>SUM(B8)</f>
-        <v>21</v>
+        <f>SUM(B8:B9)</f>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>9</v>
@@ -5203,7 +5269,7 @@
         <v>21</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5215,7 +5281,7 @@
       </c>
       <c r="D7">
         <f>D5+D6</f>
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5234,8 +5300,12 @@
         <v>21</v>
       </c>
       <c r="D9" s="25">
-        <f>D7*D3</f>
-        <v>0.29710144927536231</v>
+        <f>D7*E2</f>
+        <v>0.3282442748091603</v>
+      </c>
+      <c r="E9" s="33">
+        <f>D9</f>
+        <v>0.3282442748091603</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5289,19 +5359,19 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>[2]Ausentes!D23*'% cOB. caRT'!D9</f>
-        <v>2185.18115942029</v>
+        <v>2344.9770992366412</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="26">
         <f>A17-[2]Ausentes!E23</f>
-        <v>952.18115942028999</v>
+        <v>1117.9770992366412</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <f ca="1">TODAY()-2</f>
-        <v>45836</v>
+        <v>45838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualização de base de dados
</commit_message>
<xml_diff>
--- a/Cobertura_de_Carteira.xlsx
+++ b/Cobertura_de_Carteira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\Kidy\Documentos\kIDY - mAPEAMENTOS\cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03674C59-3EFC-4D86-BD78-A51A7DB75C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBF1B45-587B-4539-9633-5837463FF715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2BD4FA7B-4EC3-4FF7-B70D-ACBAF1B8A7C0}"/>
   </bookViews>
@@ -372,7 +372,7 @@
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="25">
     <dxf>
       <font>
         <b val="0"/>
@@ -784,40 +784,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="4" tint="-0.499984740745262"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFFC000"/>
       </font>
@@ -846,6 +812,70 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="4" tint="-0.499984740745262"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -934,7 +964,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:t>03/07/2025</a:t>
+            <a:t>06/07/2025</a:t>
           </a:fld>
           <a:endParaRPr lang="pt-BR" sz="1100" b="1">
             <a:solidFill>
@@ -1408,7 +1438,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:t>34,35%</a:t>
+            <a:t>35,11%</a:t>
           </a:fld>
           <a:endParaRPr lang="pt-BR" sz="1100" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -2321,10 +2351,10 @@
       <sheetData sheetId="6">
         <row r="23">
           <cell r="D23">
-            <v>7033</v>
+            <v>7008</v>
           </cell>
           <cell r="E23">
-            <v>1300</v>
+            <v>1326</v>
           </cell>
         </row>
       </sheetData>
@@ -2369,7 +2399,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C699080-BB77-4B73-A408-C4AABE6B398B}" name="Tabela1" displayName="Tabela1" ref="A8:M60" totalsRowCount="1" headerRowDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C699080-BB77-4B73-A408-C4AABE6B398B}" name="Tabela1" displayName="Tabela1" ref="A8:M60" totalsRowCount="1" headerRowDxfId="24" tableBorderDxfId="23">
   <autoFilter ref="A8:M59" xr:uid="{2C699080-BB77-4B73-A408-C4AABE6B398B}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{2E103CB5-8552-4DFF-8DFF-D7107D28CA72}" name="Rep" dataDxfId="16"/>
@@ -2696,8 +2726,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2731,7 +2761,7 @@
       <c r="M2" s="24"/>
       <c r="P2" s="13">
         <f ca="1">TODAY()-1</f>
-        <v>45841</v>
+        <v>45844</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2749,19 +2779,19 @@
     <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E5" s="16">
         <f>E6/D6</f>
-        <v>4.422673198040588E-2</v>
+        <v>4.8145556333100067E-2</v>
       </c>
       <c r="F5" s="16">
         <f>F6/D6</f>
-        <v>2.8691392582225334E-2</v>
+        <v>2.9111266620013995E-2</v>
       </c>
       <c r="G5" s="16">
         <f>G6/D6</f>
-        <v>2.5052484254723582E-2</v>
+        <v>2.4772568229531142E-2</v>
       </c>
       <c r="J5" s="26">
         <f>J6-'% cOB. caRT'!D9</f>
-        <v>-0.1586948453205477</v>
+        <v>-0.16195970502483717</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -2779,27 +2809,27 @@
       </c>
       <c r="E6" s="2">
         <f>SUBTOTAL(9,Tabela1[Bloqueados])</f>
-        <v>316</v>
+        <v>344</v>
       </c>
       <c r="F6" s="2">
         <f>SUBTOTAL(9,Tabela1[Abertos 2025 2º SEM])</f>
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="G6" s="2">
         <f>SUBTOTAL(9,Tabela1[Sem Limite])</f>
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H6" s="2">
         <f>SUBTOTAL(9,Tabela1[Saldo de Carteira])</f>
-        <v>7034</v>
+        <v>7009</v>
       </c>
       <c r="I6" s="2">
         <f>SUBTOTAL(9,Tabela1[cobertura])</f>
-        <v>1300</v>
+        <v>1326</v>
       </c>
       <c r="J6" s="26">
         <f>I6/H6</f>
-        <v>0.18481660506113165</v>
+        <v>0.18918533314310174</v>
       </c>
       <c r="K6" s="3">
         <f>SUBTOTAL(101,Tabela1[mix])</f>
@@ -2879,7 +2909,7 @@
         <v>142</v>
       </c>
       <c r="E9" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9" s="8">
         <v>2</v>
@@ -2889,14 +2919,14 @@
       </c>
       <c r="H9" s="8">
         <f>D9-E9+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I9" s="8">
         <v>13</v>
       </c>
       <c r="J9" s="12">
         <f t="shared" ref="J9:J59" si="0">I9/H9</f>
-        <v>9.3525179856115109E-2</v>
+        <v>9.420289855072464E-2</v>
       </c>
       <c r="K9" s="10">
         <v>14.92</v>
@@ -2904,7 +2934,7 @@
       <c r="L9" s="10"/>
       <c r="M9" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>111.2</v>
+        <v>110.4</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2925,21 +2955,21 @@
         <v>19</v>
       </c>
       <c r="F10" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G10" s="14">
         <v>6</v>
       </c>
       <c r="H10" s="8">
         <f>D10-E10+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I10" s="8">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J10" s="12">
         <f t="shared" si="0"/>
-        <v>0.32098765432098764</v>
+        <v>0.32515337423312884</v>
       </c>
       <c r="K10" s="10">
         <v>12.53</v>
@@ -2947,7 +2977,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>129.6</v>
+        <v>130.4</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -3008,7 +3038,7 @@
         <v>184</v>
       </c>
       <c r="E12" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F12" s="8">
         <v>11</v>
@@ -3018,14 +3048,14 @@
       </c>
       <c r="H12" s="8">
         <f>D12-E12+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I12" s="8">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J12" s="12">
         <f t="shared" si="0"/>
-        <v>0.34574468085106386</v>
+        <v>0.35294117647058826</v>
       </c>
       <c r="K12" s="10">
         <v>7.87</v>
@@ -3033,7 +3063,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>150.4</v>
+        <v>149.6</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3051,7 +3081,7 @@
         <v>145</v>
       </c>
       <c r="E13" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F13" s="8">
         <v>3</v>
@@ -3061,14 +3091,14 @@
       </c>
       <c r="H13" s="8">
         <f>D13-E13+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I13" s="8">
         <v>18</v>
       </c>
       <c r="J13" s="12">
         <f t="shared" si="0"/>
-        <v>0.12676056338028169</v>
+        <v>0.1276595744680851</v>
       </c>
       <c r="K13" s="10">
         <v>8.75</v>
@@ -3076,7 +3106,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>113.60000000000001</v>
+        <v>112.80000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3138,10 +3168,10 @@
         <v>144</v>
       </c>
       <c r="E15" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G15" s="14">
         <v>7</v>
@@ -3181,7 +3211,7 @@
         <v>106</v>
       </c>
       <c r="E16" s="8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" s="8">
         <v>14</v>
@@ -3191,14 +3221,14 @@
       </c>
       <c r="H16" s="8">
         <f>D16-E16+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I16" s="8">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J16" s="12">
         <f t="shared" si="0"/>
-        <v>0.29906542056074764</v>
+        <v>0.30555555555555558</v>
       </c>
       <c r="K16" s="10">
         <v>4.76</v>
@@ -3206,7 +3236,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>85.600000000000009</v>
+        <v>86.4</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -3267,7 +3297,7 @@
         <v>222</v>
       </c>
       <c r="E18" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F18" s="8">
         <v>11</v>
@@ -3277,14 +3307,14 @@
       </c>
       <c r="H18" s="8">
         <f>D18-E18+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I18" s="8">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J18" s="12">
         <f t="shared" si="0"/>
-        <v>0.30044843049327352</v>
+        <v>0.30630630630630629</v>
       </c>
       <c r="K18" s="10">
         <v>10.050000000000001</v>
@@ -3292,7 +3322,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>178.4</v>
+        <v>177.60000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3323,11 +3353,11 @@
         <v>94</v>
       </c>
       <c r="I19" s="8">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J19" s="12">
         <f t="shared" si="0"/>
-        <v>0.32978723404255317</v>
+        <v>0.34042553191489361</v>
       </c>
       <c r="K19" s="10">
         <v>4.4800000000000004</v>
@@ -3353,7 +3383,7 @@
         <v>86</v>
       </c>
       <c r="E20" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F20" s="8">
         <v>2</v>
@@ -3363,14 +3393,14 @@
       </c>
       <c r="H20" s="8">
         <f>D20-E20+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I20" s="8">
         <v>14</v>
       </c>
       <c r="J20" s="12">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>0.16867469879518071</v>
       </c>
       <c r="K20" s="10">
         <v>10</v>
@@ -3378,7 +3408,7 @@
       <c r="L20" s="10"/>
       <c r="M20" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>67.2</v>
+        <v>66.400000000000006</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3396,7 +3426,7 @@
         <v>94</v>
       </c>
       <c r="E21" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" s="8">
         <v>3</v>
@@ -3406,14 +3436,14 @@
       </c>
       <c r="H21" s="8">
         <f>D21-E21+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I21" s="8">
         <v>26</v>
       </c>
       <c r="J21" s="12">
         <f t="shared" si="0"/>
-        <v>0.27368421052631581</v>
+        <v>0.27659574468085107</v>
       </c>
       <c r="K21" s="10">
         <v>11.67</v>
@@ -3421,7 +3451,7 @@
       <c r="L21" s="10"/>
       <c r="M21" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>76</v>
+        <v>75.2</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3439,7 +3469,7 @@
         <v>159</v>
       </c>
       <c r="E22" s="8">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F22" s="8">
         <v>4</v>
@@ -3449,14 +3479,14 @@
       </c>
       <c r="H22" s="8">
         <f>D22-E22+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I22" s="8">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J22" s="12">
         <f t="shared" si="0"/>
-        <v>0.1032258064516129</v>
+        <v>0.11464968152866242</v>
       </c>
       <c r="K22" s="10">
         <v>4.82</v>
@@ -3464,7 +3494,7 @@
       <c r="L22" s="10"/>
       <c r="M22" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>124</v>
+        <v>125.60000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3483,24 +3513,24 @@
         <v>158</v>
       </c>
       <c r="E23" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F23" s="8">
         <v>8</v>
       </c>
       <c r="G23" s="14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H23" s="8">
         <f>D23-E23+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I23" s="8">
         <v>32</v>
       </c>
       <c r="J23" s="12">
         <f t="shared" si="0"/>
-        <v>0.20253164556962025</v>
+        <v>0.20512820512820512</v>
       </c>
       <c r="K23" s="10">
         <v>7.5</v>
@@ -3508,7 +3538,7 @@
       <c r="L23" s="10"/>
       <c r="M23" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>126.4</v>
+        <v>124.80000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3526,7 +3556,7 @@
         <v>229</v>
       </c>
       <c r="E24" s="8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F24" s="8">
         <v>11</v>
@@ -3536,14 +3566,14 @@
       </c>
       <c r="H24" s="8">
         <f>D24-E24+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I24" s="8">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J24" s="12">
         <f t="shared" si="0"/>
-        <v>0.24336283185840707</v>
+        <v>0.25</v>
       </c>
       <c r="K24" s="10">
         <v>9.52</v>
@@ -3551,7 +3581,7 @@
       <c r="L24" s="10"/>
       <c r="M24" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>180.8</v>
+        <v>179.20000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -3569,7 +3599,7 @@
         <v>106</v>
       </c>
       <c r="E25" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" s="8">
         <v>0</v>
@@ -3579,14 +3609,14 @@
       </c>
       <c r="H25" s="8">
         <f>D25-E25+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I25" s="8">
         <v>29</v>
       </c>
       <c r="J25" s="12">
         <f t="shared" si="0"/>
-        <v>0.28712871287128711</v>
+        <v>0.28431372549019607</v>
       </c>
       <c r="K25" s="10">
         <v>7.29</v>
@@ -3594,7 +3624,7 @@
       <c r="L25" s="10"/>
       <c r="M25" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>80.800000000000011</v>
+        <v>81.600000000000009</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3626,11 +3656,11 @@
         <v>89</v>
       </c>
       <c r="I26" s="8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J26" s="12">
         <f t="shared" si="0"/>
-        <v>0.15730337078651685</v>
+        <v>0.16853932584269662</v>
       </c>
       <c r="K26" s="10">
         <v>7.29</v>
@@ -3656,24 +3686,24 @@
         <v>119</v>
       </c>
       <c r="E27" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="8">
         <v>5</v>
       </c>
       <c r="G27" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="8">
         <f>D27-E27+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I27" s="8">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J27" s="12">
         <f t="shared" si="0"/>
-        <v>0.21951219512195122</v>
+        <v>0.22950819672131148</v>
       </c>
       <c r="K27" s="10">
         <v>8.33</v>
@@ -3681,7 +3711,7 @@
       <c r="L27" s="10"/>
       <c r="M27" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>98.4</v>
+        <v>97.600000000000009</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3698,7 +3728,7 @@
         <v>178</v>
       </c>
       <c r="E28" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F28" s="8">
         <v>5</v>
@@ -3708,14 +3738,14 @@
       </c>
       <c r="H28" s="8">
         <f>D28-E28+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I28" s="8">
         <v>53</v>
       </c>
       <c r="J28" s="12">
         <f t="shared" si="0"/>
-        <v>0.3045977011494253</v>
+        <v>0.30635838150289019</v>
       </c>
       <c r="K28" s="10">
         <v>7.33</v>
@@ -3723,7 +3753,7 @@
       <c r="L28" s="10"/>
       <c r="M28" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>139.20000000000002</v>
+        <v>138.4</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3784,7 +3814,7 @@
         <v>257</v>
       </c>
       <c r="E30" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F30" s="8">
         <v>6</v>
@@ -3794,14 +3824,14 @@
       </c>
       <c r="H30" s="8">
         <f>D30-E30+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I30" s="8">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J30" s="12">
         <f t="shared" si="0"/>
-        <v>4.6511627906976744E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="K30" s="10">
         <v>7.5</v>
@@ -3809,7 +3839,7 @@
       <c r="L30" s="10"/>
       <c r="M30" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>206.4</v>
+        <v>204.8</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -3840,11 +3870,11 @@
         <v>137</v>
       </c>
       <c r="I31" s="8">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J31" s="12">
         <f t="shared" si="0"/>
-        <v>0.29197080291970801</v>
+        <v>0.29927007299270075</v>
       </c>
       <c r="K31" s="10">
         <v>6.54</v>
@@ -3870,7 +3900,7 @@
         <v>117</v>
       </c>
       <c r="E32" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F32" s="8">
         <v>0</v>
@@ -3880,14 +3910,14 @@
       </c>
       <c r="H32" s="8">
         <f>D32-E32+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I32" s="8">
         <v>10</v>
       </c>
       <c r="J32" s="12">
         <f t="shared" si="0"/>
-        <v>8.9285714285714288E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="K32" s="10">
         <v>16.13</v>
@@ -3895,7 +3925,7 @@
       <c r="L32" s="10"/>
       <c r="M32" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>89.600000000000009</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3913,24 +3943,24 @@
         <v>260</v>
       </c>
       <c r="E33" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F33" s="8">
         <v>0</v>
       </c>
       <c r="G33" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H33" s="8">
         <f>D33-E33+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I33" s="8">
         <v>12</v>
       </c>
       <c r="J33" s="12">
         <f t="shared" si="0"/>
-        <v>4.6875E-2</v>
+        <v>4.7058823529411764E-2</v>
       </c>
       <c r="K33" s="10">
         <v>5.88</v>
@@ -3938,7 +3968,7 @@
       <c r="L33" s="10"/>
       <c r="M33" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>204.8</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3956,7 +3986,7 @@
         <v>177</v>
       </c>
       <c r="E34" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F34" s="8">
         <v>5</v>
@@ -3966,14 +3996,14 @@
       </c>
       <c r="H34" s="8">
         <f>D34-E34+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I34" s="8">
         <v>42</v>
       </c>
       <c r="J34" s="12">
         <f t="shared" si="0"/>
-        <v>0.23728813559322035</v>
+        <v>0.23863636363636365</v>
       </c>
       <c r="K34" s="10">
         <v>6.59</v>
@@ -3981,7 +4011,7 @@
       <c r="L34" s="10"/>
       <c r="M34" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>141.6</v>
+        <v>140.80000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3999,7 +4029,7 @@
         <v>122</v>
       </c>
       <c r="E35" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F35" s="8">
         <v>1</v>
@@ -4009,14 +4039,14 @@
       </c>
       <c r="H35" s="8">
         <f>D35-E35+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I35" s="8">
         <v>44</v>
       </c>
       <c r="J35" s="12">
         <f t="shared" si="0"/>
-        <v>0.38596491228070173</v>
+        <v>0.38938053097345132</v>
       </c>
       <c r="K35" s="10">
         <v>8.8699999999999992</v>
@@ -4024,7 +4054,7 @@
       <c r="L35" s="10"/>
       <c r="M35" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>91.2</v>
+        <v>90.4</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4042,7 +4072,7 @@
         <v>272</v>
       </c>
       <c r="E36" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F36" s="8">
         <v>4</v>
@@ -4052,14 +4082,14 @@
       </c>
       <c r="H36" s="8">
         <f>D36-E36+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="I36" s="8">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J36" s="12">
         <f t="shared" si="0"/>
-        <v>0.15730337078651685</v>
+        <v>0.16417910447761194</v>
       </c>
       <c r="K36" s="10">
         <v>10.37</v>
@@ -4067,7 +4097,7 @@
       <c r="L36" s="10"/>
       <c r="M36" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>213.60000000000002</v>
+        <v>214.4</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4091,18 +4121,18 @@
         <v>4</v>
       </c>
       <c r="G37" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H37" s="8">
         <f>D37-E37+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
         <v>172</v>
       </c>
       <c r="I37" s="8">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J37" s="12">
         <f t="shared" si="0"/>
-        <v>0.11046511627906977</v>
+        <v>0.13372093023255813</v>
       </c>
       <c r="K37" s="10">
         <v>4.93</v>
@@ -4127,7 +4157,7 @@
         <v>134</v>
       </c>
       <c r="E38" s="8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F38" s="8">
         <v>0</v>
@@ -4137,14 +4167,14 @@
       </c>
       <c r="H38" s="8">
         <f>D38-E38+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I38" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J38" s="12">
         <f t="shared" si="0"/>
-        <v>8.2644628099173556E-2</v>
+        <v>9.166666666666666E-2</v>
       </c>
       <c r="K38" s="10">
         <v>6</v>
@@ -4152,7 +4182,7 @@
       <c r="L38" s="10"/>
       <c r="M38" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>96.800000000000011</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4183,11 +4213,11 @@
         <v>163</v>
       </c>
       <c r="I39" s="8">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J39" s="12">
         <f t="shared" si="0"/>
-        <v>0.21472392638036811</v>
+        <v>0.22085889570552147</v>
       </c>
       <c r="K39" s="10">
         <v>6.23</v>
@@ -4213,7 +4243,7 @@
         <v>214</v>
       </c>
       <c r="E40" s="8">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F40" s="8">
         <v>2</v>
@@ -4223,14 +4253,14 @@
       </c>
       <c r="H40" s="8">
         <f>D40-E40+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I40" s="8">
         <v>20</v>
       </c>
       <c r="J40" s="12">
         <f t="shared" si="0"/>
-        <v>9.8522167487684734E-2</v>
+        <v>0.1</v>
       </c>
       <c r="K40" s="10">
         <v>7.69</v>
@@ -4238,7 +4268,7 @@
       <c r="L40" s="10"/>
       <c r="M40" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>162.4</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4256,7 +4286,7 @@
         <v>130</v>
       </c>
       <c r="E41" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F41" s="8">
         <v>3</v>
@@ -4266,14 +4296,14 @@
       </c>
       <c r="H41" s="8">
         <f>D41-E41+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I41" s="8">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J41" s="12">
         <f t="shared" si="0"/>
-        <v>0.2109375</v>
+        <v>0.2283464566929134</v>
       </c>
       <c r="K41" s="10">
         <v>8.8699999999999992</v>
@@ -4281,7 +4311,7 @@
       <c r="L41" s="10"/>
       <c r="M41" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>102.4</v>
+        <v>101.60000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4300,7 +4330,7 @@
         <v>79</v>
       </c>
       <c r="E42" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42" s="8">
         <v>2</v>
@@ -4310,14 +4340,14 @@
       </c>
       <c r="H42" s="8">
         <f>D42-E42+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I42" s="8">
         <v>6</v>
       </c>
       <c r="J42" s="12">
         <f t="shared" si="0"/>
-        <v>7.5949367088607597E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="K42" s="10">
         <v>8.17</v>
@@ -4325,7 +4355,7 @@
       <c r="L42" s="10"/>
       <c r="M42" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>63.2</v>
+        <v>62.400000000000006</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4342,7 +4372,7 @@
         <v>206</v>
       </c>
       <c r="E43" s="8">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F43" s="8">
         <v>0</v>
@@ -4352,14 +4382,14 @@
       </c>
       <c r="H43" s="8">
         <f>D43-E43+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I43" s="8">
         <v>20</v>
       </c>
       <c r="J43" s="12">
         <f t="shared" si="0"/>
-        <v>0.12048192771084337</v>
+        <v>0.12121212121212122</v>
       </c>
       <c r="K43" s="10">
         <v>6.65</v>
@@ -4367,7 +4397,7 @@
       <c r="L43" s="10"/>
       <c r="M43" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>132.80000000000001</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4471,7 +4501,7 @@
         <v>103</v>
       </c>
       <c r="E46" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F46" s="8">
         <v>0</v>
@@ -4481,14 +4511,14 @@
       </c>
       <c r="H46" s="8">
         <f>D46-E46+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I46" s="8">
         <v>17</v>
       </c>
       <c r="J46" s="12">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>0.16831683168316833</v>
       </c>
       <c r="K46" s="10">
         <v>5.92</v>
@@ -4496,7 +4526,7 @@
       <c r="L46" s="10"/>
       <c r="M46" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>81.600000000000009</v>
+        <v>80.800000000000011</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -4555,7 +4585,7 @@
         <v>147</v>
       </c>
       <c r="E48" s="8">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F48" s="8">
         <v>3</v>
@@ -4565,14 +4595,14 @@
       </c>
       <c r="H48" s="8">
         <f>D48-E48+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I48" s="8">
         <v>13</v>
       </c>
       <c r="J48" s="12">
         <f t="shared" si="0"/>
-        <v>0.10743801652892562</v>
+        <v>0.10833333333333334</v>
       </c>
       <c r="K48" s="10">
         <v>7.3</v>
@@ -4580,7 +4610,7 @@
       <c r="L48" s="10"/>
       <c r="M48" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>96.800000000000011</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -4598,24 +4628,24 @@
         <v>117</v>
       </c>
       <c r="E49" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F49" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G49" s="14">
         <v>2</v>
       </c>
       <c r="H49" s="8">
         <f>D49-E49+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I49" s="8">
         <v>33</v>
       </c>
       <c r="J49" s="12">
         <f t="shared" si="0"/>
-        <v>0.27500000000000002</v>
+        <v>0.27731092436974791</v>
       </c>
       <c r="K49" s="10">
         <v>5.19</v>
@@ -4623,7 +4653,7 @@
       <c r="L49" s="10"/>
       <c r="M49" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>96</v>
+        <v>95.2</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4641,7 +4671,7 @@
         <v>136</v>
       </c>
       <c r="E50" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="8">
         <v>5</v>
@@ -4651,14 +4681,14 @@
       </c>
       <c r="H50" s="8">
         <f>D50-E50+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I50" s="8">
         <v>24</v>
       </c>
       <c r="J50" s="12">
         <f t="shared" si="0"/>
-        <v>0.1702127659574468</v>
+        <v>0.17142857142857143</v>
       </c>
       <c r="K50" s="10">
         <v>7.4</v>
@@ -4666,7 +4696,7 @@
       <c r="L50" s="10"/>
       <c r="M50" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>112.80000000000001</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4685,7 +4715,7 @@
         <v>94</v>
       </c>
       <c r="E51" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F51" s="8">
         <v>17</v>
@@ -4695,14 +4725,14 @@
       </c>
       <c r="H51" s="8">
         <f>D51-E51+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I51" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J51" s="12">
         <f t="shared" si="0"/>
-        <v>4.5454545454545456E-2</v>
+        <v>5.5045871559633031E-2</v>
       </c>
       <c r="K51" s="10">
         <v>15</v>
@@ -4710,7 +4740,7 @@
       <c r="L51" s="10"/>
       <c r="M51" s="27">
         <f>Tabela1[[#This Row],[Saldo de Carteira]]*80%</f>
-        <v>88</v>
+        <v>87.2</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4942,7 +4972,7 @@
         <v>20</v>
       </c>
       <c r="G57" s="14">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H57" s="8">
         <f>D57-E57+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
@@ -5026,7 +5056,7 @@
         <v>4</v>
       </c>
       <c r="G59" s="14">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H59" s="8">
         <f>D59-E59+Tabela1[[#This Row],[Abertos 2025 2º SEM]]</f>
@@ -5063,16 +5093,16 @@
   </mergeCells>
   <conditionalFormatting sqref="J1:J1048576">
     <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
-      <formula>0.3435</formula>
+      <formula>0.3511</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J60">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThan">
       <formula>0.1699</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="between">
       <formula>0.17</formula>
-      <formula>0.3434</formula>
+      <formula>0.341</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:L59">
@@ -5166,7 +5196,7 @@
       </c>
       <c r="D3" s="23">
         <f>E2*D7</f>
-        <v>0.34351145038167935</v>
+        <v>0.35114503816793891</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5203,7 +5233,7 @@
         <v>21</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5215,7 +5245,7 @@
       </c>
       <c r="D7">
         <f>D5+D6</f>
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5235,11 +5265,11 @@
       </c>
       <c r="D9" s="23">
         <f>D7*E2</f>
-        <v>0.34351145038167935</v>
+        <v>0.35114503816793891</v>
       </c>
       <c r="E9" s="31">
         <f>D9</f>
-        <v>0.34351145038167935</v>
+        <v>0.35114503816793891</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5293,19 +5323,19 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>[2]Ausentes!D23*'% cOB. caRT'!D9</f>
-        <v>2415.9160305343507</v>
+        <v>2460.8244274809158</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <f>A17-[2]Ausentes!E23</f>
-        <v>1115.9160305343507</v>
+        <v>1134.8244274809158</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="25">
         <f ca="1">TODAY()-2</f>
-        <v>45840</v>
+        <v>45843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>